<commit_message>
laatste audio aanpassingen voor de demo op 23-05-2017
</commit_message>
<xml_diff>
--- a/Steps_code_and_files/Beweegdata/Beweegdata_Steps.xlsx
+++ b/Steps_code_and_files/Beweegdata/Beweegdata_Steps.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>Datum</t>
   </si>
@@ -34,85 +34,58 @@
     <t>Afgerond</t>
   </si>
   <si>
-    <t>01-05-2017</t>
-  </si>
-  <si>
-    <t>10:17</t>
+    <t>07-04-2017</t>
+  </si>
+  <si>
+    <t>12:40</t>
   </si>
   <si>
     <t>Knie extensie</t>
   </si>
   <si>
-    <t>10:30</t>
+    <t>11-05-2017</t>
+  </si>
+  <si>
+    <t>09:39</t>
+  </si>
+  <si>
+    <t>Been heffen</t>
+  </si>
+  <si>
+    <t>09:52</t>
+  </si>
+  <si>
+    <t>13:38</t>
+  </si>
+  <si>
+    <t>13:45</t>
+  </si>
+  <si>
+    <t>13:53</t>
+  </si>
+  <si>
+    <t>16:13</t>
+  </si>
+  <si>
+    <t>Achteren lopen</t>
+  </si>
+  <si>
+    <t>09-05-2017</t>
+  </si>
+  <si>
+    <t>15:34</t>
   </si>
   <si>
     <t>Staan zitten</t>
   </si>
   <si>
-    <t>11:32</t>
-  </si>
-  <si>
-    <t>Achteren lopen</t>
-  </si>
-  <si>
-    <t>11:35</t>
-  </si>
-  <si>
-    <t>08-05-2017</t>
-  </si>
-  <si>
-    <t>12:15</t>
-  </si>
-  <si>
-    <t>12:16</t>
-  </si>
-  <si>
-    <t>11:21</t>
-  </si>
-  <si>
-    <t>11:24</t>
-  </si>
-  <si>
-    <t>09-05-2017</t>
-  </si>
-  <si>
-    <t>13:11</t>
-  </si>
-  <si>
-    <t>13:13</t>
-  </si>
-  <si>
-    <t>17-05-2017</t>
-  </si>
-  <si>
-    <t>22:27</t>
-  </si>
-  <si>
-    <t>Op 1 been staan</t>
-  </si>
-  <si>
-    <t>22:37</t>
-  </si>
-  <si>
-    <t>22:41</t>
-  </si>
-  <si>
-    <t>22:48</t>
+    <t>22-05-2017</t>
+  </si>
+  <si>
+    <t>15:36</t>
   </si>
   <si>
     <t>Leunen naar grond</t>
-  </si>
-  <si>
-    <t>22:49</t>
-  </si>
-  <si>
-    <t>Knien optillen</t>
-  </si>
-  <si>
-    <t>22:52</t>
-  </si>
-  <si>
-    <t>22:53</t>
   </si>
 </sst>
 </file>
@@ -503,7 +476,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E8" activeCellId="0" pane="topLeft" sqref="E8"/>
@@ -550,318 +523,156 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.000120227974537037</v>
+        <v>0.001076547384259259</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F2" s="4" t="n"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.001301096516203704</v>
+        <v>0.0005314786226851851</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F3" s="5" t="n"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" s="3" t="n">
-        <v>0.001845518113425926</v>
+        <v>0.0005008594097222223</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F4" s="5" t="n"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>0.001462120335648148</v>
+        <v>0.0004975766087962964</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F5" s="5" t="n"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>0.0005222168402777777</v>
+        <v>0.0002537568634259259</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F6" s="5" t="n"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.0001630247569444444</v>
+        <v>0.002010784664351852</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4" t="n"/>
+        <v>3</v>
+      </c>
+      <c r="F7" s="5" t="n"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
       <c r="D8" s="3" t="n">
-        <v>0.001560717465277778</v>
+        <v>0.0004963550810185185</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5" t="n"/>
+        <v>4</v>
+      </c>
+      <c r="F8" s="4" t="n"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>0.001387439930555555</v>
+        <v>0.0002644919328703704</v>
       </c>
       <c r="E9" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4" t="n"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>0.002496182662037037</v>
+        <v>0.0002566921064814814</v>
       </c>
       <c r="E10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F10" s="5" t="n"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>0.0685162586574074</v>
-      </c>
-      <c r="E11" t="n">
-        <v>8</v>
-      </c>
-      <c r="F11" s="4" t="n"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>0.0009357454398148148</v>
-      </c>
-      <c r="E12" t="n">
         <v>6</v>
       </c>
-      <c r="F12" s="4" t="n"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="3" t="n">
-        <v>0.0002998422685185185</v>
-      </c>
-      <c r="E13" t="n">
-        <v>10</v>
-      </c>
-      <c r="F13" s="4" t="n"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="3" t="n">
-        <v>0.00234970337962963</v>
-      </c>
-      <c r="E14" t="n">
-        <v>10</v>
-      </c>
-      <c r="F14" s="5" t="n"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="3" t="n">
-        <v>0.001653966284722222</v>
-      </c>
-      <c r="E15" t="n">
-        <v>10</v>
-      </c>
-      <c r="F15" s="5" t="n"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="3" t="n">
-        <v>0.003908018518518519</v>
-      </c>
-      <c r="E16" t="n">
-        <v>20</v>
-      </c>
-      <c r="F16" s="5" t="n"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>0.0002291874074074074</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="4" t="n"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="3" t="n">
-        <v>0.001118592604166667</v>
-      </c>
-      <c r="E18" t="n">
-        <v>10</v>
-      </c>
-      <c r="F18" s="5" t="n"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="3" t="n">
-        <v>5.151393518518518e-05</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="4" t="n"/>
+      <c r="F10" s="4" t="n"/>
     </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>

</xml_diff>

<commit_message>
small changes in handen tikken
</commit_message>
<xml_diff>
--- a/Steps_code_and_files/Beweegdata/Beweegdata_Steps.xlsx
+++ b/Steps_code_and_files/Beweegdata/Beweegdata_Steps.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Datum</t>
   </si>
@@ -47,6 +47,39 @@
   </si>
   <si>
     <t>Hak naar bil</t>
+  </si>
+  <si>
+    <t>14-06-2017</t>
+  </si>
+  <si>
+    <t>10:36</t>
+  </si>
+  <si>
+    <t>Knie extensie</t>
+  </si>
+  <si>
+    <t>10:37</t>
+  </si>
+  <si>
+    <t>Leunen naar grond</t>
+  </si>
+  <si>
+    <t>Naar voren leunen</t>
+  </si>
+  <si>
+    <t>10:59</t>
+  </si>
+  <si>
+    <t>Knien optillen</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>Knien en handen optillen</t>
+  </si>
+  <si>
+    <t>Beide benen strekken</t>
   </si>
 </sst>
 </file>
@@ -430,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E8" activeCellId="0" pane="topLeft" sqref="E8"/>
@@ -438,12 +471,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.6" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="2" min="1" width="11.5204081632653"/>
-    <col customWidth="1" max="3" min="3" width="21.8061224489796"/>
-    <col customWidth="1" max="4" min="4" width="12.6785714285714"/>
-    <col customWidth="1" max="5" min="5" width="19.6275510204082"/>
-    <col customWidth="1" max="6" min="6" width="8.79081632653061"/>
-    <col customWidth="1" max="1025" min="7" width="11.5204081632653"/>
+    <col customWidth="1" max="2" min="1" style="2" width="11.5204081632653"/>
+    <col customWidth="1" max="3" min="3" style="2" width="21.8061224489796"/>
+    <col customWidth="1" max="4" min="4" style="2" width="12.6785714285714"/>
+    <col customWidth="1" max="5" min="5" style="2" width="19.6275510204082"/>
+    <col customWidth="1" max="6" min="6" style="2" width="8.79081632653061"/>
+    <col customWidth="1" max="1025" min="7" style="2" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="13.6" r="1" s="2" spans="1:6">
@@ -501,6 +534,114 @@
         <v>0</v>
       </c>
       <c r="F3" s="4" t="n"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0.0002199911226851852</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="n"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0.0001773612615740741</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="n"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>5.244998842592592e-05</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="n"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0.01494191704861111</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4" t="n"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>5.223804398148148e-05</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="n"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>5.206115740740741e-05</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="n"/>
     </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>

</xml_diff>